<commit_message>
[AndroidUpdate] ResultActivity 주석 수정
</commit_message>
<xml_diff>
--- a/PREZENTAINER_error.xlsx
+++ b/PREZENTAINER_error.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>index</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -117,6 +117,36 @@
   <si>
     <t>어플이 종료 되었음에도 
 FileTransferRequestedActivity의 변수가 저장이 되어있다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Unterminated object at character</t>
+  </si>
+  <si>
+    <t>08-29-00:10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IndexOutOfBoudsException</t>
+  </si>
+  <si>
+    <t>08-25-17:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>size-1 보다 큰 Index를 참조 하였기 때문에 생긴 에러</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JSON Object에서 "right" -&gt; 'right' , "left" -&gt; 'left'</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -453,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -573,6 +603,40 @@
         <v>20</v>
       </c>
     </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[AndroidUpdate] 이름 중복 해결
</commit_message>
<xml_diff>
--- a/PREZENTAINER_error.xlsx
+++ b/PREZENTAINER_error.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
   <si>
     <t>index</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -125,6 +125,165 @@
   </si>
   <si>
     <t>Gear 측 어플이 자동으로 꺼짐</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>08-31-16:33</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>clearInterval(vibratingInterval); 해줬음에도 타이머가 다시 울림</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JSON 파싱 Error : Unterminated object at character</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>09-01-12:03</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>JSON으로 인식을 못해서 character를 못 읽는 것이다.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+JSON Object형태의 데이터를 String으로 만드는 과정에서 
+"{"right" : [10,20] , "left" : [20,30]}" value값의 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 가 문제가되었다.
+즉, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>""</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">내부에 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">를 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>\"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 이나 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 로 바꿔줘야한다.</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -135,7 +294,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="mm&quot;월&quot;\ dd&quot;일&quot;"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -148,6 +307,23 @@
       <sz val="8"/>
       <name val="맑은 고딕"/>
       <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
@@ -174,7 +350,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -186,6 +362,9 @@
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -467,10 +646,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -601,8 +780,40 @@
         <v>6</v>
       </c>
     </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="66" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>